<commit_message>
ajout des dependances pour les vibrations, video, et implementation des features
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningJeudiVendredi.xlsx
+++ b/documentation/3_2_Modele_PlanningJeudiVendredi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/leon_fejzaj_studentfr_ch/Documents/011.EMF (EXERCICE)/3eme annee (2025-2026)/306/306-G3-SpeleoThink/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D7E285-1E25-49E2-9A7D-4133DDA9F5BF}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30AD2C4A-7A2D-47B7-860F-715E75ECC380}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3600" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Tâches</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>Websummary</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -1153,148 +1156,148 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1348,13 +1351,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19843</xdr:colOff>
+      <xdr:colOff>19842</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>139212</xdr:colOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>7326</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>8282</xdr:rowOff>
     </xdr:to>
@@ -1371,8 +1374,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3866478" y="688731"/>
-          <a:ext cx="5101676" cy="2448147"/>
+          <a:off x="3866477" y="688731"/>
+          <a:ext cx="6288637" cy="2448147"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1433,10 +1436,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1793,7 +1792,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1809,12 +1808,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1857,177 +1856,177 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:85" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="96"/>
-      <c r="X2" s="96"/>
-      <c r="Y2" s="96"/>
-      <c r="Z2" s="96"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="96"/>
-      <c r="AD2" s="96"/>
-      <c r="AE2" s="96"/>
-      <c r="AF2" s="96"/>
-      <c r="AG2" s="96"/>
-      <c r="AH2" s="96"/>
-      <c r="AI2" s="96"/>
-      <c r="AJ2" s="96"/>
-      <c r="AK2" s="96"/>
-      <c r="AL2" s="96"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="96"/>
-      <c r="AO2" s="96"/>
-      <c r="AP2" s="96"/>
-      <c r="AQ2" s="96"/>
-      <c r="AR2" s="96"/>
-      <c r="AS2" s="96"/>
-      <c r="AT2" s="96"/>
-      <c r="AU2" s="96"/>
-      <c r="AV2" s="96"/>
-      <c r="AW2" s="96"/>
-      <c r="AX2" s="96"/>
-      <c r="AY2" s="96"/>
-      <c r="AZ2" s="96"/>
-      <c r="BA2" s="96"/>
-      <c r="BB2" s="96"/>
-      <c r="BC2" s="96"/>
-      <c r="BD2" s="96"/>
-      <c r="BE2" s="96"/>
-      <c r="BF2" s="96"/>
-      <c r="BG2" s="96"/>
-      <c r="BH2" s="96"/>
-      <c r="BI2" s="96"/>
-      <c r="BJ2" s="96"/>
-      <c r="BK2" s="96"/>
-      <c r="BL2" s="96"/>
-      <c r="BM2" s="96"/>
-      <c r="BN2" s="96"/>
-      <c r="BO2" s="96"/>
-      <c r="BP2" s="96"/>
-      <c r="BQ2" s="96"/>
-      <c r="BR2" s="96"/>
-      <c r="BS2" s="96"/>
-      <c r="BT2" s="96"/>
-      <c r="BU2" s="96"/>
-      <c r="BV2" s="96"/>
-      <c r="BW2" s="96"/>
-      <c r="BX2" s="96"/>
-      <c r="BY2" s="96"/>
-      <c r="BZ2" s="96"/>
-      <c r="CA2" s="96"/>
-      <c r="CB2" s="96"/>
-      <c r="CC2" s="96"/>
-      <c r="CD2" s="96"/>
-      <c r="CE2" s="96"/>
-      <c r="CF2" s="96"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="122"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="122"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="122"/>
+      <c r="AA2" s="122"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="122"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="122"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="122"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="122"/>
+      <c r="AK2" s="122"/>
+      <c r="AL2" s="122"/>
+      <c r="AM2" s="122"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="122"/>
+      <c r="AP2" s="122"/>
+      <c r="AQ2" s="122"/>
+      <c r="AR2" s="122"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="122"/>
+      <c r="AU2" s="122"/>
+      <c r="AV2" s="122"/>
+      <c r="AW2" s="122"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="122"/>
+      <c r="AZ2" s="122"/>
+      <c r="BA2" s="122"/>
+      <c r="BB2" s="122"/>
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="122"/>
+      <c r="BF2" s="122"/>
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="122"/>
+      <c r="BQ2" s="122"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="122"/>
+      <c r="BV2" s="122"/>
+      <c r="BW2" s="122"/>
+      <c r="BX2" s="122"/>
+      <c r="BY2" s="122"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="122"/>
+      <c r="CB2" s="122"/>
+      <c r="CC2" s="122"/>
+      <c r="CD2" s="122"/>
+      <c r="CE2" s="122"/>
+      <c r="CF2" s="122"/>
     </row>
     <row r="3" spans="1:85" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="97"/>
-      <c r="AF3" s="97"/>
-      <c r="AG3" s="97"/>
-      <c r="AH3" s="97"/>
-      <c r="AI3" s="97"/>
-      <c r="AJ3" s="97"/>
-      <c r="AK3" s="97"/>
-      <c r="AL3" s="97"/>
-      <c r="AM3" s="97"/>
-      <c r="AN3" s="97"/>
-      <c r="AO3" s="97"/>
-      <c r="AP3" s="97"/>
-      <c r="AQ3" s="97"/>
-      <c r="AR3" s="97"/>
-      <c r="AS3" s="97"/>
-      <c r="AT3" s="97"/>
-      <c r="AU3" s="97"/>
-      <c r="AV3" s="97"/>
-      <c r="AW3" s="97"/>
-      <c r="AX3" s="97"/>
-      <c r="AY3" s="97"/>
-      <c r="AZ3" s="97"/>
-      <c r="BA3" s="97"/>
-      <c r="BB3" s="97"/>
-      <c r="BC3" s="97"/>
-      <c r="BD3" s="97"/>
-      <c r="BE3" s="97"/>
-      <c r="BF3" s="97"/>
-      <c r="BG3" s="97"/>
-      <c r="BH3" s="97"/>
-      <c r="BI3" s="97"/>
-      <c r="BJ3" s="97"/>
-      <c r="BK3" s="97"/>
-      <c r="BL3" s="97"/>
-      <c r="BM3" s="97"/>
-      <c r="BN3" s="97"/>
-      <c r="BO3" s="97"/>
-      <c r="BP3" s="97"/>
-      <c r="BQ3" s="97"/>
-      <c r="BR3" s="97"/>
-      <c r="BS3" s="97"/>
-      <c r="BT3" s="97"/>
-      <c r="BU3" s="97"/>
-      <c r="BV3" s="97"/>
-      <c r="BW3" s="97"/>
-      <c r="BX3" s="97"/>
-      <c r="BY3" s="97"/>
-      <c r="BZ3" s="97"/>
-      <c r="CA3" s="97"/>
-      <c r="CB3" s="97"/>
-      <c r="CC3" s="97"/>
-      <c r="CD3" s="97"/>
-      <c r="CE3" s="97"/>
-      <c r="CF3" s="97"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
+      <c r="Q3" s="123"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="123"/>
+      <c r="U3" s="123"/>
+      <c r="V3" s="123"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+      <c r="Y3" s="123"/>
+      <c r="Z3" s="123"/>
+      <c r="AA3" s="123"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="123"/>
+      <c r="AE3" s="123"/>
+      <c r="AF3" s="123"/>
+      <c r="AG3" s="123"/>
+      <c r="AH3" s="123"/>
+      <c r="AI3" s="123"/>
+      <c r="AJ3" s="123"/>
+      <c r="AK3" s="123"/>
+      <c r="AL3" s="123"/>
+      <c r="AM3" s="123"/>
+      <c r="AN3" s="123"/>
+      <c r="AO3" s="123"/>
+      <c r="AP3" s="123"/>
+      <c r="AQ3" s="123"/>
+      <c r="AR3" s="123"/>
+      <c r="AS3" s="123"/>
+      <c r="AT3" s="123"/>
+      <c r="AU3" s="123"/>
+      <c r="AV3" s="123"/>
+      <c r="AW3" s="123"/>
+      <c r="AX3" s="123"/>
+      <c r="AY3" s="123"/>
+      <c r="AZ3" s="123"/>
+      <c r="BA3" s="123"/>
+      <c r="BB3" s="123"/>
+      <c r="BC3" s="123"/>
+      <c r="BD3" s="123"/>
+      <c r="BE3" s="123"/>
+      <c r="BF3" s="123"/>
+      <c r="BG3" s="123"/>
+      <c r="BH3" s="123"/>
+      <c r="BI3" s="123"/>
+      <c r="BJ3" s="123"/>
+      <c r="BK3" s="123"/>
+      <c r="BL3" s="123"/>
+      <c r="BM3" s="123"/>
+      <c r="BN3" s="123"/>
+      <c r="BO3" s="123"/>
+      <c r="BP3" s="123"/>
+      <c r="BQ3" s="123"/>
+      <c r="BR3" s="123"/>
+      <c r="BS3" s="123"/>
+      <c r="BT3" s="123"/>
+      <c r="BU3" s="123"/>
+      <c r="BV3" s="123"/>
+      <c r="BW3" s="123"/>
+      <c r="BX3" s="123"/>
+      <c r="BY3" s="123"/>
+      <c r="BZ3" s="123"/>
+      <c r="CA3" s="123"/>
+      <c r="CB3" s="123"/>
+      <c r="CC3" s="123"/>
+      <c r="CD3" s="123"/>
+      <c r="CE3" s="123"/>
+      <c r="CF3" s="123"/>
     </row>
     <row r="4" spans="1:85" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="105" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="11"/>
@@ -2037,132 +2036,132 @@
       <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="92">
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109">
         <v>45995</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="94" t="s">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="92">
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="109">
         <v>45996</v>
       </c>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="94" t="s">
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="110"/>
+      <c r="U4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="95"/>
-      <c r="W4" s="95"/>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="92">
+      <c r="V4" s="108"/>
+      <c r="W4" s="108"/>
+      <c r="X4" s="108"/>
+      <c r="Y4" s="109">
         <v>46002</v>
       </c>
-      <c r="Z4" s="92"/>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93"/>
-      <c r="AC4" s="94" t="s">
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="110"/>
+      <c r="AC4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="92">
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="109">
         <v>46003</v>
       </c>
-      <c r="AH4" s="92"/>
-      <c r="AI4" s="92"/>
-      <c r="AJ4" s="93"/>
-      <c r="AK4" s="94" t="s">
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="110"/>
+      <c r="AK4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="95"/>
-      <c r="AM4" s="95"/>
-      <c r="AN4" s="95"/>
-      <c r="AO4" s="92">
+      <c r="AL4" s="108"/>
+      <c r="AM4" s="108"/>
+      <c r="AN4" s="108"/>
+      <c r="AO4" s="109">
         <v>46009</v>
       </c>
-      <c r="AP4" s="92"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="93"/>
-      <c r="AS4" s="94" t="s">
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="110"/>
+      <c r="AS4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="AT4" s="95"/>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="92">
+      <c r="AT4" s="108"/>
+      <c r="AU4" s="108"/>
+      <c r="AV4" s="108"/>
+      <c r="AW4" s="109">
         <v>46010</v>
       </c>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="92"/>
-      <c r="AZ4" s="93"/>
-      <c r="BA4" s="94" t="s">
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109"/>
+      <c r="AZ4" s="110"/>
+      <c r="BA4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="92">
+      <c r="BB4" s="108"/>
+      <c r="BC4" s="108"/>
+      <c r="BD4" s="108"/>
+      <c r="BE4" s="109">
         <v>46030</v>
       </c>
-      <c r="BF4" s="92"/>
-      <c r="BG4" s="92"/>
-      <c r="BH4" s="93"/>
-      <c r="BI4" s="94" t="s">
+      <c r="BF4" s="109"/>
+      <c r="BG4" s="109"/>
+      <c r="BH4" s="110"/>
+      <c r="BI4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="BJ4" s="95"/>
-      <c r="BK4" s="95"/>
-      <c r="BL4" s="95"/>
-      <c r="BM4" s="92">
+      <c r="BJ4" s="108"/>
+      <c r="BK4" s="108"/>
+      <c r="BL4" s="108"/>
+      <c r="BM4" s="109">
         <v>46031</v>
       </c>
-      <c r="BN4" s="92"/>
-      <c r="BO4" s="92"/>
-      <c r="BP4" s="93"/>
-      <c r="BQ4" s="94" t="s">
+      <c r="BN4" s="109"/>
+      <c r="BO4" s="109"/>
+      <c r="BP4" s="110"/>
+      <c r="BQ4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="BR4" s="95"/>
-      <c r="BS4" s="95"/>
-      <c r="BT4" s="95"/>
-      <c r="BU4" s="92">
+      <c r="BR4" s="108"/>
+      <c r="BS4" s="108"/>
+      <c r="BT4" s="108"/>
+      <c r="BU4" s="109">
         <v>46037</v>
       </c>
-      <c r="BV4" s="92"/>
-      <c r="BW4" s="92"/>
-      <c r="BX4" s="93"/>
-      <c r="BY4" s="94" t="s">
+      <c r="BV4" s="109"/>
+      <c r="BW4" s="109"/>
+      <c r="BX4" s="110"/>
+      <c r="BY4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="BZ4" s="95"/>
-      <c r="CA4" s="95"/>
-      <c r="CB4" s="95"/>
-      <c r="CC4" s="92">
+      <c r="BZ4" s="108"/>
+      <c r="CA4" s="108"/>
+      <c r="CB4" s="108"/>
+      <c r="CC4" s="109">
         <v>46038</v>
       </c>
-      <c r="CD4" s="92"/>
-      <c r="CE4" s="92"/>
-      <c r="CF4" s="93"/>
-      <c r="CG4" s="112" t="s">
+      <c r="CD4" s="109"/>
+      <c r="CE4" s="109"/>
+      <c r="CF4" s="110"/>
+      <c r="CG4" s="103" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:85" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="115"/>
+      <c r="A5" s="106"/>
       <c r="B5" s="12"/>
       <c r="C5" s="8" t="s">
         <v>3</v>
@@ -2410,10 +2409,10 @@
       <c r="CF5" s="6">
         <v>8</v>
       </c>
-      <c r="CG5" s="112"/>
+      <c r="CG5" s="103"/>
     </row>
     <row r="6" spans="1:85" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="111" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -2423,12 +2422,12 @@
         <v>13</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="100" t="s">
+      <c r="E6" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="102"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="93"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
@@ -2441,16 +2440,16 @@
       <c r="R6" s="16"/>
       <c r="S6" s="16"/>
       <c r="T6" s="34"/>
-      <c r="U6" s="122" t="s">
+      <c r="U6" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="123"/>
-      <c r="Y6" s="123"/>
-      <c r="Z6" s="123"/>
-      <c r="AA6" s="123"/>
-      <c r="AB6" s="123"/>
+      <c r="V6" s="118"/>
+      <c r="W6" s="118"/>
+      <c r="X6" s="118"/>
+      <c r="Y6" s="118"/>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="118"/>
+      <c r="AB6" s="118"/>
       <c r="AC6" s="37"/>
       <c r="AD6" s="16"/>
       <c r="AE6" s="16"/>
@@ -2459,12 +2458,12 @@
       <c r="AH6" s="16"/>
       <c r="AI6" s="16"/>
       <c r="AJ6" s="17"/>
-      <c r="AK6" s="100" t="s">
+      <c r="AK6" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="AL6" s="101"/>
-      <c r="AM6" s="101"/>
-      <c r="AN6" s="102"/>
+      <c r="AL6" s="92"/>
+      <c r="AM6" s="92"/>
+      <c r="AN6" s="93"/>
       <c r="AO6" s="21"/>
       <c r="AP6" s="21"/>
       <c r="AQ6" s="21"/>
@@ -2477,12 +2476,12 @@
       <c r="AX6" s="16"/>
       <c r="AY6" s="16"/>
       <c r="AZ6" s="17"/>
-      <c r="BA6" s="109" t="s">
+      <c r="BA6" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="BB6" s="110"/>
-      <c r="BC6" s="110"/>
-      <c r="BD6" s="111"/>
+      <c r="BB6" s="101"/>
+      <c r="BC6" s="101"/>
+      <c r="BD6" s="102"/>
       <c r="BE6" s="16"/>
       <c r="BF6" s="16"/>
       <c r="BG6" s="16"/>
@@ -2495,12 +2494,12 @@
       <c r="BN6" s="16"/>
       <c r="BO6" s="16"/>
       <c r="BP6" s="17"/>
-      <c r="BQ6" s="100" t="s">
+      <c r="BQ6" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="BR6" s="101"/>
-      <c r="BS6" s="101"/>
-      <c r="BT6" s="102"/>
+      <c r="BR6" s="92"/>
+      <c r="BS6" s="92"/>
+      <c r="BT6" s="93"/>
       <c r="BU6" s="16"/>
       <c r="BV6" s="16"/>
       <c r="BW6" s="16"/>
@@ -2513,10 +2512,10 @@
       <c r="CD6" s="16"/>
       <c r="CE6" s="16"/>
       <c r="CF6" s="17"/>
-      <c r="CG6" s="112"/>
+      <c r="CG6" s="103"/>
     </row>
     <row r="7" spans="1:85" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
+      <c r="A7" s="112"/>
       <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
@@ -2524,10 +2523,10 @@
         <v>13</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="105"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="96"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
@@ -2540,14 +2539,14 @@
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="35"/>
-      <c r="U7" s="123"/>
-      <c r="V7" s="123"/>
-      <c r="W7" s="123"/>
-      <c r="X7" s="123"/>
-      <c r="Y7" s="123"/>
-      <c r="Z7" s="123"/>
-      <c r="AA7" s="123"/>
-      <c r="AB7" s="123"/>
+      <c r="U7" s="118"/>
+      <c r="V7" s="118"/>
+      <c r="W7" s="118"/>
+      <c r="X7" s="118"/>
+      <c r="Y7" s="118"/>
+      <c r="Z7" s="118"/>
+      <c r="AA7" s="118"/>
+      <c r="AB7" s="118"/>
       <c r="AC7" s="38"/>
       <c r="AD7" s="21"/>
       <c r="AE7" s="21"/>
@@ -2556,10 +2555,10 @@
       <c r="AH7" s="21"/>
       <c r="AI7" s="21"/>
       <c r="AJ7" s="22"/>
-      <c r="AK7" s="103"/>
-      <c r="AL7" s="104"/>
-      <c r="AM7" s="104"/>
-      <c r="AN7" s="105"/>
+      <c r="AK7" s="94"/>
+      <c r="AL7" s="95"/>
+      <c r="AM7" s="95"/>
+      <c r="AN7" s="96"/>
       <c r="AO7" s="21"/>
       <c r="AP7" s="21"/>
       <c r="AQ7" s="21"/>
@@ -2572,10 +2571,10 @@
       <c r="AX7" s="21"/>
       <c r="AY7" s="21"/>
       <c r="AZ7" s="22"/>
-      <c r="BA7" s="103"/>
-      <c r="BB7" s="104"/>
-      <c r="BC7" s="104"/>
-      <c r="BD7" s="105"/>
+      <c r="BA7" s="94"/>
+      <c r="BB7" s="95"/>
+      <c r="BC7" s="95"/>
+      <c r="BD7" s="96"/>
       <c r="BE7" s="21"/>
       <c r="BF7" s="21"/>
       <c r="BG7" s="21"/>
@@ -2588,10 +2587,10 @@
       <c r="BN7" s="21"/>
       <c r="BO7" s="21"/>
       <c r="BP7" s="22"/>
-      <c r="BQ7" s="103"/>
-      <c r="BR7" s="104"/>
-      <c r="BS7" s="104"/>
-      <c r="BT7" s="105"/>
+      <c r="BQ7" s="94"/>
+      <c r="BR7" s="95"/>
+      <c r="BS7" s="95"/>
+      <c r="BT7" s="96"/>
       <c r="BU7" s="21"/>
       <c r="BV7" s="21"/>
       <c r="BW7" s="21"/>
@@ -2604,10 +2603,10 @@
       <c r="CD7" s="21"/>
       <c r="CE7" s="21"/>
       <c r="CF7" s="22"/>
-      <c r="CG7" s="112"/>
+      <c r="CG7" s="103"/>
     </row>
     <row r="8" spans="1:85" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="13" t="s">
         <v>15</v>
       </c>
@@ -2615,10 +2614,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="105"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="96"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
@@ -2631,14 +2630,14 @@
       <c r="R8" s="33"/>
       <c r="S8" s="21"/>
       <c r="T8" s="35"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="123"/>
-      <c r="Y8" s="123"/>
-      <c r="Z8" s="123"/>
-      <c r="AA8" s="123"/>
-      <c r="AB8" s="123"/>
+      <c r="U8" s="118"/>
+      <c r="V8" s="118"/>
+      <c r="W8" s="118"/>
+      <c r="X8" s="118"/>
+      <c r="Y8" s="118"/>
+      <c r="Z8" s="118"/>
+      <c r="AA8" s="118"/>
+      <c r="AB8" s="118"/>
       <c r="AC8" s="38"/>
       <c r="AD8" s="21"/>
       <c r="AE8" s="21"/>
@@ -2647,10 +2646,10 @@
       <c r="AH8" s="21"/>
       <c r="AI8" s="21"/>
       <c r="AJ8" s="22"/>
-      <c r="AK8" s="103"/>
-      <c r="AL8" s="104"/>
-      <c r="AM8" s="104"/>
-      <c r="AN8" s="105"/>
+      <c r="AK8" s="94"/>
+      <c r="AL8" s="95"/>
+      <c r="AM8" s="95"/>
+      <c r="AN8" s="96"/>
       <c r="AO8" s="21"/>
       <c r="AP8" s="21"/>
       <c r="AQ8" s="21"/>
@@ -2663,10 +2662,10 @@
       <c r="AX8" s="21"/>
       <c r="AY8" s="21"/>
       <c r="AZ8" s="22"/>
-      <c r="BA8" s="103"/>
-      <c r="BB8" s="104"/>
-      <c r="BC8" s="104"/>
-      <c r="BD8" s="105"/>
+      <c r="BA8" s="94"/>
+      <c r="BB8" s="95"/>
+      <c r="BC8" s="95"/>
+      <c r="BD8" s="96"/>
       <c r="BE8" s="21"/>
       <c r="BF8" s="21"/>
       <c r="BG8" s="21"/>
@@ -2679,10 +2678,10 @@
       <c r="BN8" s="21"/>
       <c r="BO8" s="21"/>
       <c r="BP8" s="22"/>
-      <c r="BQ8" s="103"/>
-      <c r="BR8" s="104"/>
-      <c r="BS8" s="104"/>
-      <c r="BT8" s="105"/>
+      <c r="BQ8" s="94"/>
+      <c r="BR8" s="95"/>
+      <c r="BS8" s="95"/>
+      <c r="BT8" s="96"/>
       <c r="BU8" s="21"/>
       <c r="BV8" s="21"/>
       <c r="BW8" s="21"/>
@@ -2695,10 +2694,10 @@
       <c r="CD8" s="21"/>
       <c r="CE8" s="21"/>
       <c r="CF8" s="22"/>
-      <c r="CG8" s="112"/>
+      <c r="CG8" s="103"/>
     </row>
     <row r="9" spans="1:85" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="114" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -2708,10 +2707,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="26"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="105"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="96"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
@@ -2724,14 +2723,14 @@
       <c r="R9" s="28"/>
       <c r="S9" s="33"/>
       <c r="T9" s="84"/>
-      <c r="U9" s="123"/>
-      <c r="V9" s="123"/>
-      <c r="W9" s="123"/>
-      <c r="X9" s="123"/>
-      <c r="Y9" s="123"/>
-      <c r="Z9" s="123"/>
-      <c r="AA9" s="123"/>
-      <c r="AB9" s="123"/>
+      <c r="U9" s="118"/>
+      <c r="V9" s="118"/>
+      <c r="W9" s="118"/>
+      <c r="X9" s="118"/>
+      <c r="Y9" s="118"/>
+      <c r="Z9" s="118"/>
+      <c r="AA9" s="118"/>
+      <c r="AB9" s="118"/>
       <c r="AC9" s="39"/>
       <c r="AD9" s="28"/>
       <c r="AE9" s="28"/>
@@ -2740,10 +2739,10 @@
       <c r="AH9" s="28"/>
       <c r="AI9" s="28"/>
       <c r="AJ9" s="29"/>
-      <c r="AK9" s="103"/>
-      <c r="AL9" s="104"/>
-      <c r="AM9" s="104"/>
-      <c r="AN9" s="105"/>
+      <c r="AK9" s="94"/>
+      <c r="AL9" s="95"/>
+      <c r="AM9" s="95"/>
+      <c r="AN9" s="96"/>
       <c r="AO9" s="28"/>
       <c r="AP9" s="28"/>
       <c r="AQ9" s="28"/>
@@ -2756,10 +2755,10 @@
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="29"/>
-      <c r="BA9" s="103"/>
-      <c r="BB9" s="104"/>
-      <c r="BC9" s="104"/>
-      <c r="BD9" s="105"/>
+      <c r="BA9" s="94"/>
+      <c r="BB9" s="95"/>
+      <c r="BC9" s="95"/>
+      <c r="BD9" s="96"/>
       <c r="BE9" s="28"/>
       <c r="BF9" s="28"/>
       <c r="BG9" s="28"/>
@@ -2772,10 +2771,10 @@
       <c r="BN9" s="28"/>
       <c r="BO9" s="28"/>
       <c r="BP9" s="29"/>
-      <c r="BQ9" s="103"/>
-      <c r="BR9" s="104"/>
-      <c r="BS9" s="104"/>
-      <c r="BT9" s="105"/>
+      <c r="BQ9" s="94"/>
+      <c r="BR9" s="95"/>
+      <c r="BS9" s="95"/>
+      <c r="BT9" s="96"/>
       <c r="BU9" s="28"/>
       <c r="BV9" s="28"/>
       <c r="BW9" s="28"/>
@@ -2788,10 +2787,10 @@
       <c r="CD9" s="28"/>
       <c r="CE9" s="28"/>
       <c r="CF9" s="29"/>
-      <c r="CG9" s="112"/>
+      <c r="CG9" s="103"/>
     </row>
     <row r="10" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A10" s="120"/>
+      <c r="A10" s="115"/>
       <c r="B10" s="24" t="s">
         <v>18</v>
       </c>
@@ -2799,10 +2798,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="26"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="96"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
@@ -2815,14 +2814,14 @@
       <c r="R10" s="28"/>
       <c r="S10" s="33"/>
       <c r="T10" s="84"/>
-      <c r="U10" s="123"/>
-      <c r="V10" s="123"/>
-      <c r="W10" s="123"/>
-      <c r="X10" s="123"/>
-      <c r="Y10" s="123"/>
-      <c r="Z10" s="123"/>
-      <c r="AA10" s="123"/>
-      <c r="AB10" s="123"/>
+      <c r="U10" s="118"/>
+      <c r="V10" s="118"/>
+      <c r="W10" s="118"/>
+      <c r="X10" s="118"/>
+      <c r="Y10" s="118"/>
+      <c r="Z10" s="118"/>
+      <c r="AA10" s="118"/>
+      <c r="AB10" s="118"/>
       <c r="AC10" s="39"/>
       <c r="AD10" s="28"/>
       <c r="AE10" s="28"/>
@@ -2831,10 +2830,10 @@
       <c r="AH10" s="28"/>
       <c r="AI10" s="28"/>
       <c r="AJ10" s="29"/>
-      <c r="AK10" s="103"/>
-      <c r="AL10" s="104"/>
-      <c r="AM10" s="104"/>
-      <c r="AN10" s="105"/>
+      <c r="AK10" s="94"/>
+      <c r="AL10" s="95"/>
+      <c r="AM10" s="95"/>
+      <c r="AN10" s="96"/>
       <c r="AO10" s="28"/>
       <c r="AP10" s="28"/>
       <c r="AQ10" s="28"/>
@@ -2847,10 +2846,10 @@
       <c r="AX10" s="28"/>
       <c r="AY10" s="28"/>
       <c r="AZ10" s="29"/>
-      <c r="BA10" s="103"/>
-      <c r="BB10" s="104"/>
-      <c r="BC10" s="104"/>
-      <c r="BD10" s="105"/>
+      <c r="BA10" s="94"/>
+      <c r="BB10" s="95"/>
+      <c r="BC10" s="95"/>
+      <c r="BD10" s="96"/>
       <c r="BE10" s="28"/>
       <c r="BF10" s="28"/>
       <c r="BG10" s="28"/>
@@ -2863,10 +2862,10 @@
       <c r="BN10" s="28"/>
       <c r="BO10" s="28"/>
       <c r="BP10" s="29"/>
-      <c r="BQ10" s="103"/>
-      <c r="BR10" s="104"/>
-      <c r="BS10" s="104"/>
-      <c r="BT10" s="105"/>
+      <c r="BQ10" s="94"/>
+      <c r="BR10" s="95"/>
+      <c r="BS10" s="95"/>
+      <c r="BT10" s="96"/>
       <c r="BU10" s="28"/>
       <c r="BV10" s="28"/>
       <c r="BW10" s="28"/>
@@ -2879,10 +2878,10 @@
       <c r="CD10" s="28"/>
       <c r="CE10" s="28"/>
       <c r="CF10" s="29"/>
-      <c r="CG10" s="112"/>
+      <c r="CG10" s="103"/>
     </row>
     <row r="11" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A11" s="121"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="24" t="s">
         <v>19</v>
       </c>
@@ -2890,10 +2889,10 @@
         <v>13</v>
       </c>
       <c r="D11" s="26"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="105"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="96"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
@@ -2906,14 +2905,14 @@
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="36"/>
-      <c r="U11" s="123"/>
-      <c r="V11" s="123"/>
-      <c r="W11" s="123"/>
-      <c r="X11" s="123"/>
-      <c r="Y11" s="123"/>
-      <c r="Z11" s="123"/>
-      <c r="AA11" s="123"/>
-      <c r="AB11" s="123"/>
+      <c r="U11" s="118"/>
+      <c r="V11" s="118"/>
+      <c r="W11" s="118"/>
+      <c r="X11" s="118"/>
+      <c r="Y11" s="118"/>
+      <c r="Z11" s="118"/>
+      <c r="AA11" s="118"/>
+      <c r="AB11" s="118"/>
       <c r="AC11" s="88"/>
       <c r="AD11" s="33"/>
       <c r="AE11" s="28"/>
@@ -2922,10 +2921,10 @@
       <c r="AH11" s="28"/>
       <c r="AI11" s="28"/>
       <c r="AJ11" s="29"/>
-      <c r="AK11" s="103"/>
-      <c r="AL11" s="104"/>
-      <c r="AM11" s="104"/>
-      <c r="AN11" s="105"/>
+      <c r="AK11" s="94"/>
+      <c r="AL11" s="95"/>
+      <c r="AM11" s="95"/>
+      <c r="AN11" s="96"/>
       <c r="AO11" s="28"/>
       <c r="AP11" s="28"/>
       <c r="AQ11" s="28"/>
@@ -2938,10 +2937,10 @@
       <c r="AX11" s="28"/>
       <c r="AY11" s="28"/>
       <c r="AZ11" s="29"/>
-      <c r="BA11" s="103"/>
-      <c r="BB11" s="104"/>
-      <c r="BC11" s="104"/>
-      <c r="BD11" s="105"/>
+      <c r="BA11" s="94"/>
+      <c r="BB11" s="95"/>
+      <c r="BC11" s="95"/>
+      <c r="BD11" s="96"/>
       <c r="BE11" s="28"/>
       <c r="BF11" s="28"/>
       <c r="BG11" s="28"/>
@@ -2954,10 +2953,10 @@
       <c r="BN11" s="28"/>
       <c r="BO11" s="28"/>
       <c r="BP11" s="29"/>
-      <c r="BQ11" s="103"/>
-      <c r="BR11" s="104"/>
-      <c r="BS11" s="104"/>
-      <c r="BT11" s="105"/>
+      <c r="BQ11" s="94"/>
+      <c r="BR11" s="95"/>
+      <c r="BS11" s="95"/>
+      <c r="BT11" s="96"/>
       <c r="BU11" s="28"/>
       <c r="BV11" s="28"/>
       <c r="BW11" s="28"/>
@@ -2970,7 +2969,7 @@
       <c r="CD11" s="28"/>
       <c r="CE11" s="28"/>
       <c r="CF11" s="29"/>
-      <c r="CG11" s="112"/>
+      <c r="CG11" s="103"/>
     </row>
     <row r="12" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
@@ -2983,10 +2982,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="51"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="105"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="96"/>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
@@ -2999,14 +2998,14 @@
       <c r="R12" s="44"/>
       <c r="S12" s="44"/>
       <c r="T12" s="48"/>
-      <c r="U12" s="123"/>
-      <c r="V12" s="123"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="123"/>
-      <c r="Y12" s="123"/>
-      <c r="Z12" s="123"/>
-      <c r="AA12" s="123"/>
-      <c r="AB12" s="123"/>
+      <c r="U12" s="118"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="118"/>
+      <c r="X12" s="118"/>
+      <c r="Y12" s="118"/>
+      <c r="Z12" s="118"/>
+      <c r="AA12" s="118"/>
+      <c r="AB12" s="118"/>
       <c r="AC12" s="47"/>
       <c r="AD12" s="44"/>
       <c r="AE12" s="33"/>
@@ -3015,10 +3014,10 @@
       <c r="AH12" s="33"/>
       <c r="AI12" s="33"/>
       <c r="AJ12" s="89"/>
-      <c r="AK12" s="103"/>
-      <c r="AL12" s="104"/>
-      <c r="AM12" s="104"/>
-      <c r="AN12" s="105"/>
+      <c r="AK12" s="94"/>
+      <c r="AL12" s="95"/>
+      <c r="AM12" s="95"/>
+      <c r="AN12" s="96"/>
       <c r="AO12" s="44"/>
       <c r="AP12" s="44"/>
       <c r="AQ12" s="44"/>
@@ -3031,10 +3030,10 @@
       <c r="AX12" s="44"/>
       <c r="AY12" s="44"/>
       <c r="AZ12" s="45"/>
-      <c r="BA12" s="103"/>
-      <c r="BB12" s="104"/>
-      <c r="BC12" s="104"/>
-      <c r="BD12" s="105"/>
+      <c r="BA12" s="94"/>
+      <c r="BB12" s="95"/>
+      <c r="BC12" s="95"/>
+      <c r="BD12" s="96"/>
       <c r="BE12" s="44"/>
       <c r="BF12" s="44"/>
       <c r="BG12" s="44"/>
@@ -3047,10 +3046,10 @@
       <c r="BN12" s="44"/>
       <c r="BO12" s="44"/>
       <c r="BP12" s="45"/>
-      <c r="BQ12" s="103"/>
-      <c r="BR12" s="104"/>
-      <c r="BS12" s="104"/>
-      <c r="BT12" s="105"/>
+      <c r="BQ12" s="94"/>
+      <c r="BR12" s="95"/>
+      <c r="BS12" s="95"/>
+      <c r="BT12" s="96"/>
       <c r="BU12" s="44"/>
       <c r="BV12" s="44"/>
       <c r="BW12" s="44"/>
@@ -3063,7 +3062,7 @@
       <c r="CD12" s="44"/>
       <c r="CE12" s="44"/>
       <c r="CF12" s="45"/>
-      <c r="CG12" s="112"/>
+      <c r="CG12" s="103"/>
     </row>
     <row r="13" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
@@ -3072,12 +3071,14 @@
       <c r="B13" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="53"/>
+      <c r="C13" s="53" t="s">
+        <v>13</v>
+      </c>
       <c r="D13" s="54"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="105"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="96"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
@@ -3090,14 +3091,14 @@
       <c r="R13" s="56"/>
       <c r="S13" s="56"/>
       <c r="T13" s="58"/>
-      <c r="U13" s="123"/>
-      <c r="V13" s="123"/>
-      <c r="W13" s="123"/>
-      <c r="X13" s="123"/>
-      <c r="Y13" s="123"/>
-      <c r="Z13" s="123"/>
-      <c r="AA13" s="123"/>
-      <c r="AB13" s="123"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
+      <c r="W13" s="118"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="118"/>
+      <c r="Z13" s="118"/>
+      <c r="AA13" s="118"/>
+      <c r="AB13" s="118"/>
       <c r="AC13" s="59"/>
       <c r="AD13" s="56"/>
       <c r="AE13" s="56"/>
@@ -3106,10 +3107,10 @@
       <c r="AH13" s="56"/>
       <c r="AI13" s="56"/>
       <c r="AJ13" s="57"/>
-      <c r="AK13" s="103"/>
-      <c r="AL13" s="104"/>
-      <c r="AM13" s="104"/>
-      <c r="AN13" s="105"/>
+      <c r="AK13" s="94"/>
+      <c r="AL13" s="95"/>
+      <c r="AM13" s="95"/>
+      <c r="AN13" s="96"/>
       <c r="AO13" s="33"/>
       <c r="AP13" s="33"/>
       <c r="AQ13" s="33"/>
@@ -3122,10 +3123,10 @@
       <c r="AX13" s="33"/>
       <c r="AY13" s="33"/>
       <c r="AZ13" s="89"/>
-      <c r="BA13" s="103"/>
-      <c r="BB13" s="104"/>
-      <c r="BC13" s="104"/>
-      <c r="BD13" s="105"/>
+      <c r="BA13" s="94"/>
+      <c r="BB13" s="95"/>
+      <c r="BC13" s="95"/>
+      <c r="BD13" s="96"/>
       <c r="BE13" s="56"/>
       <c r="BF13" s="56"/>
       <c r="BG13" s="56"/>
@@ -3138,10 +3139,10 @@
       <c r="BN13" s="56"/>
       <c r="BO13" s="56"/>
       <c r="BP13" s="57"/>
-      <c r="BQ13" s="103"/>
-      <c r="BR13" s="104"/>
-      <c r="BS13" s="104"/>
-      <c r="BT13" s="105"/>
+      <c r="BQ13" s="94"/>
+      <c r="BR13" s="95"/>
+      <c r="BS13" s="95"/>
+      <c r="BT13" s="96"/>
       <c r="BU13" s="56"/>
       <c r="BV13" s="56"/>
       <c r="BW13" s="56"/>
@@ -3154,7 +3155,7 @@
       <c r="CD13" s="56"/>
       <c r="CE13" s="56"/>
       <c r="CF13" s="57"/>
-      <c r="CG13" s="112"/>
+      <c r="CG13" s="103"/>
     </row>
     <row r="14" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A14" s="87" t="s">
@@ -3163,12 +3164,14 @@
       <c r="B14" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="61"/>
+      <c r="C14" s="61" t="s">
+        <v>30</v>
+      </c>
       <c r="D14" s="62"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="96"/>
       <c r="I14" s="64"/>
       <c r="J14" s="64"/>
       <c r="K14" s="64"/>
@@ -3181,14 +3184,14 @@
       <c r="R14" s="64"/>
       <c r="S14" s="64"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="123"/>
-      <c r="V14" s="123"/>
-      <c r="W14" s="123"/>
-      <c r="X14" s="123"/>
-      <c r="Y14" s="123"/>
-      <c r="Z14" s="123"/>
-      <c r="AA14" s="123"/>
-      <c r="AB14" s="123"/>
+      <c r="U14" s="118"/>
+      <c r="V14" s="118"/>
+      <c r="W14" s="118"/>
+      <c r="X14" s="118"/>
+      <c r="Y14" s="118"/>
+      <c r="Z14" s="118"/>
+      <c r="AA14" s="118"/>
+      <c r="AB14" s="118"/>
       <c r="AC14" s="67"/>
       <c r="AD14" s="64"/>
       <c r="AE14" s="64"/>
@@ -3197,10 +3200,10 @@
       <c r="AH14" s="64"/>
       <c r="AI14" s="64"/>
       <c r="AJ14" s="65"/>
-      <c r="AK14" s="103"/>
-      <c r="AL14" s="104"/>
-      <c r="AM14" s="104"/>
-      <c r="AN14" s="105"/>
+      <c r="AK14" s="94"/>
+      <c r="AL14" s="95"/>
+      <c r="AM14" s="95"/>
+      <c r="AN14" s="96"/>
       <c r="AO14" s="64"/>
       <c r="AP14" s="64"/>
       <c r="AQ14" s="64"/>
@@ -3213,10 +3216,10 @@
       <c r="AX14" s="64"/>
       <c r="AY14" s="64"/>
       <c r="AZ14" s="65"/>
-      <c r="BA14" s="103"/>
-      <c r="BB14" s="104"/>
-      <c r="BC14" s="104"/>
-      <c r="BD14" s="105"/>
+      <c r="BA14" s="94"/>
+      <c r="BB14" s="95"/>
+      <c r="BC14" s="95"/>
+      <c r="BD14" s="96"/>
       <c r="BE14" s="33"/>
       <c r="BF14" s="33"/>
       <c r="BG14" s="33"/>
@@ -3229,10 +3232,10 @@
       <c r="BN14" s="33"/>
       <c r="BO14" s="33"/>
       <c r="BP14" s="89"/>
-      <c r="BQ14" s="103"/>
-      <c r="BR14" s="104"/>
-      <c r="BS14" s="104"/>
-      <c r="BT14" s="105"/>
+      <c r="BQ14" s="94"/>
+      <c r="BR14" s="95"/>
+      <c r="BS14" s="95"/>
+      <c r="BT14" s="96"/>
       <c r="BU14" s="64"/>
       <c r="BV14" s="64"/>
       <c r="BW14" s="64"/>
@@ -3245,7 +3248,7 @@
       <c r="CD14" s="64"/>
       <c r="CE14" s="64"/>
       <c r="CF14" s="65"/>
-      <c r="CG14" s="112"/>
+      <c r="CG14" s="103"/>
     </row>
     <row r="15" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A15" s="71" t="s">
@@ -3256,10 +3259,10 @@
       </c>
       <c r="C15" s="69"/>
       <c r="D15" s="70"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="105"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
       <c r="I15" s="72"/>
       <c r="J15" s="72"/>
       <c r="K15" s="72"/>
@@ -3272,14 +3275,14 @@
       <c r="R15" s="72"/>
       <c r="S15" s="72"/>
       <c r="T15" s="74"/>
-      <c r="U15" s="123"/>
-      <c r="V15" s="123"/>
-      <c r="W15" s="123"/>
-      <c r="X15" s="123"/>
-      <c r="Y15" s="123"/>
-      <c r="Z15" s="123"/>
-      <c r="AA15" s="123"/>
-      <c r="AB15" s="123"/>
+      <c r="U15" s="118"/>
+      <c r="V15" s="118"/>
+      <c r="W15" s="118"/>
+      <c r="X15" s="118"/>
+      <c r="Y15" s="118"/>
+      <c r="Z15" s="118"/>
+      <c r="AA15" s="118"/>
+      <c r="AB15" s="118"/>
       <c r="AC15" s="75"/>
       <c r="AD15" s="72"/>
       <c r="AE15" s="72"/>
@@ -3288,10 +3291,10 @@
       <c r="AH15" s="72"/>
       <c r="AI15" s="72"/>
       <c r="AJ15" s="73"/>
-      <c r="AK15" s="103"/>
-      <c r="AL15" s="104"/>
-      <c r="AM15" s="104"/>
-      <c r="AN15" s="105"/>
+      <c r="AK15" s="94"/>
+      <c r="AL15" s="95"/>
+      <c r="AM15" s="95"/>
+      <c r="AN15" s="96"/>
       <c r="AO15" s="72"/>
       <c r="AP15" s="72"/>
       <c r="AQ15" s="72"/>
@@ -3304,10 +3307,10 @@
       <c r="AX15" s="72"/>
       <c r="AY15" s="72"/>
       <c r="AZ15" s="73"/>
-      <c r="BA15" s="103"/>
-      <c r="BB15" s="104"/>
-      <c r="BC15" s="104"/>
-      <c r="BD15" s="105"/>
+      <c r="BA15" s="94"/>
+      <c r="BB15" s="95"/>
+      <c r="BC15" s="95"/>
+      <c r="BD15" s="96"/>
       <c r="BE15" s="72"/>
       <c r="BF15" s="72"/>
       <c r="BG15" s="72"/>
@@ -3320,10 +3323,10 @@
       <c r="BN15" s="72"/>
       <c r="BO15" s="72"/>
       <c r="BP15" s="73"/>
-      <c r="BQ15" s="103"/>
-      <c r="BR15" s="104"/>
-      <c r="BS15" s="104"/>
-      <c r="BT15" s="105"/>
+      <c r="BQ15" s="94"/>
+      <c r="BR15" s="95"/>
+      <c r="BS15" s="95"/>
+      <c r="BT15" s="96"/>
       <c r="BU15" s="33"/>
       <c r="BV15" s="33"/>
       <c r="BW15" s="33"/>
@@ -3336,10 +3339,10 @@
       <c r="CD15" s="72"/>
       <c r="CE15" s="72"/>
       <c r="CF15" s="73"/>
-      <c r="CG15" s="112"/>
+      <c r="CG15" s="103"/>
     </row>
     <row r="16" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="119" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="76" t="s">
@@ -3347,10 +3350,10 @@
       </c>
       <c r="C16" s="77"/>
       <c r="D16" s="78"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
       <c r="I16" s="80"/>
       <c r="J16" s="80"/>
       <c r="K16" s="80"/>
@@ -3363,14 +3366,14 @@
       <c r="R16" s="80"/>
       <c r="S16" s="80"/>
       <c r="T16" s="82"/>
-      <c r="U16" s="123"/>
-      <c r="V16" s="123"/>
-      <c r="W16" s="123"/>
-      <c r="X16" s="123"/>
-      <c r="Y16" s="123"/>
-      <c r="Z16" s="123"/>
-      <c r="AA16" s="123"/>
-      <c r="AB16" s="123"/>
+      <c r="U16" s="118"/>
+      <c r="V16" s="118"/>
+      <c r="W16" s="118"/>
+      <c r="X16" s="118"/>
+      <c r="Y16" s="118"/>
+      <c r="Z16" s="118"/>
+      <c r="AA16" s="118"/>
+      <c r="AB16" s="118"/>
       <c r="AC16" s="80"/>
       <c r="AD16" s="80"/>
       <c r="AE16" s="80"/>
@@ -3379,10 +3382,10 @@
       <c r="AH16" s="80"/>
       <c r="AI16" s="80"/>
       <c r="AJ16" s="80"/>
-      <c r="AK16" s="103"/>
-      <c r="AL16" s="104"/>
-      <c r="AM16" s="104"/>
-      <c r="AN16" s="105"/>
+      <c r="AK16" s="94"/>
+      <c r="AL16" s="95"/>
+      <c r="AM16" s="95"/>
+      <c r="AN16" s="96"/>
       <c r="AO16" s="80"/>
       <c r="AP16" s="80"/>
       <c r="AQ16" s="80"/>
@@ -3395,10 +3398,10 @@
       <c r="AX16" s="80"/>
       <c r="AY16" s="80"/>
       <c r="AZ16" s="80"/>
-      <c r="BA16" s="103"/>
-      <c r="BB16" s="104"/>
-      <c r="BC16" s="104"/>
-      <c r="BD16" s="105"/>
+      <c r="BA16" s="94"/>
+      <c r="BB16" s="95"/>
+      <c r="BC16" s="95"/>
+      <c r="BD16" s="96"/>
       <c r="BE16" s="80"/>
       <c r="BF16" s="80"/>
       <c r="BG16" s="80"/>
@@ -3411,10 +3414,10 @@
       <c r="BN16" s="80"/>
       <c r="BO16" s="80"/>
       <c r="BP16" s="80"/>
-      <c r="BQ16" s="103"/>
-      <c r="BR16" s="104"/>
-      <c r="BS16" s="104"/>
-      <c r="BT16" s="105"/>
+      <c r="BQ16" s="94"/>
+      <c r="BR16" s="95"/>
+      <c r="BS16" s="95"/>
+      <c r="BT16" s="96"/>
       <c r="BU16" s="80"/>
       <c r="BV16" s="80"/>
       <c r="BW16" s="80"/>
@@ -3427,10 +3430,10 @@
       <c r="CD16" s="80"/>
       <c r="CE16" s="80"/>
       <c r="CF16" s="80"/>
-      <c r="CG16" s="112"/>
+      <c r="CG16" s="103"/>
     </row>
     <row r="17" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A17" s="125"/>
+      <c r="A17" s="120"/>
       <c r="B17" s="76" t="s">
         <v>28</v>
       </c>
@@ -3516,10 +3519,10 @@
       <c r="CD17" s="33"/>
       <c r="CE17" s="80"/>
       <c r="CF17" s="80"/>
-      <c r="CG17" s="112"/>
+      <c r="CG17" s="103"/>
     </row>
     <row r="18" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A18" s="126"/>
+      <c r="A18" s="121"/>
       <c r="B18" s="76" t="s">
         <v>29</v>
       </c>
@@ -3605,153 +3608,173 @@
       <c r="CD18" s="80"/>
       <c r="CE18" s="33"/>
       <c r="CF18" s="33"/>
-      <c r="CG18" s="112"/>
+      <c r="CG18" s="103"/>
     </row>
     <row r="19" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="113"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="113"/>
-      <c r="O19" s="113"/>
-      <c r="P19" s="113"/>
-      <c r="Q19" s="113"/>
-      <c r="R19" s="113"/>
-      <c r="S19" s="113"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="113"/>
-      <c r="V19" s="113"/>
-      <c r="W19" s="113"/>
-      <c r="X19" s="113"/>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="113"/>
-      <c r="AA19" s="113"/>
-      <c r="AB19" s="113"/>
-      <c r="AC19" s="113"/>
-      <c r="AD19" s="113"/>
-      <c r="AE19" s="113"/>
-      <c r="AF19" s="113"/>
-      <c r="AG19" s="113"/>
-      <c r="AH19" s="113"/>
-      <c r="AI19" s="113"/>
-      <c r="AJ19" s="113"/>
-      <c r="AK19" s="113"/>
-      <c r="AL19" s="113"/>
-      <c r="AM19" s="113"/>
-      <c r="AN19" s="113"/>
-      <c r="AO19" s="113"/>
-      <c r="AP19" s="113"/>
-      <c r="AQ19" s="113"/>
-      <c r="AR19" s="113"/>
-      <c r="AS19" s="113"/>
-      <c r="AT19" s="113"/>
-      <c r="AU19" s="113"/>
-      <c r="AV19" s="113"/>
-      <c r="AW19" s="113"/>
-      <c r="AX19" s="113"/>
-      <c r="AY19" s="113"/>
-      <c r="AZ19" s="113"/>
-      <c r="BA19" s="113"/>
-      <c r="BB19" s="113"/>
-      <c r="BC19" s="113"/>
-      <c r="BD19" s="113"/>
-      <c r="BE19" s="113"/>
-      <c r="BF19" s="113"/>
-      <c r="BG19" s="113"/>
-      <c r="BH19" s="113"/>
-      <c r="BI19" s="113"/>
-      <c r="BJ19" s="113"/>
-      <c r="BK19" s="113"/>
-      <c r="BL19" s="113"/>
-      <c r="BM19" s="113"/>
-      <c r="BN19" s="113"/>
-      <c r="BO19" s="113"/>
-      <c r="BP19" s="113"/>
-      <c r="BQ19" s="113"/>
-      <c r="BR19" s="113"/>
-      <c r="BS19" s="113"/>
-      <c r="BT19" s="113"/>
-      <c r="BU19" s="113"/>
-      <c r="BV19" s="113"/>
-      <c r="BW19" s="113"/>
-      <c r="BX19" s="113"/>
-      <c r="BY19" s="113"/>
-      <c r="BZ19" s="113"/>
-      <c r="CA19" s="113"/>
-      <c r="CB19" s="113"/>
-      <c r="CC19" s="113"/>
-      <c r="CD19" s="113"/>
-      <c r="CE19" s="113"/>
-      <c r="CF19" s="113"/>
-      <c r="CG19" s="112"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="104"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
+      <c r="T19" s="104"/>
+      <c r="U19" s="104"/>
+      <c r="V19" s="104"/>
+      <c r="W19" s="104"/>
+      <c r="X19" s="104"/>
+      <c r="Y19" s="104"/>
+      <c r="Z19" s="104"/>
+      <c r="AA19" s="104"/>
+      <c r="AB19" s="104"/>
+      <c r="AC19" s="104"/>
+      <c r="AD19" s="104"/>
+      <c r="AE19" s="104"/>
+      <c r="AF19" s="104"/>
+      <c r="AG19" s="104"/>
+      <c r="AH19" s="104"/>
+      <c r="AI19" s="104"/>
+      <c r="AJ19" s="104"/>
+      <c r="AK19" s="104"/>
+      <c r="AL19" s="104"/>
+      <c r="AM19" s="104"/>
+      <c r="AN19" s="104"/>
+      <c r="AO19" s="104"/>
+      <c r="AP19" s="104"/>
+      <c r="AQ19" s="104"/>
+      <c r="AR19" s="104"/>
+      <c r="AS19" s="104"/>
+      <c r="AT19" s="104"/>
+      <c r="AU19" s="104"/>
+      <c r="AV19" s="104"/>
+      <c r="AW19" s="104"/>
+      <c r="AX19" s="104"/>
+      <c r="AY19" s="104"/>
+      <c r="AZ19" s="104"/>
+      <c r="BA19" s="104"/>
+      <c r="BB19" s="104"/>
+      <c r="BC19" s="104"/>
+      <c r="BD19" s="104"/>
+      <c r="BE19" s="104"/>
+      <c r="BF19" s="104"/>
+      <c r="BG19" s="104"/>
+      <c r="BH19" s="104"/>
+      <c r="BI19" s="104"/>
+      <c r="BJ19" s="104"/>
+      <c r="BK19" s="104"/>
+      <c r="BL19" s="104"/>
+      <c r="BM19" s="104"/>
+      <c r="BN19" s="104"/>
+      <c r="BO19" s="104"/>
+      <c r="BP19" s="104"/>
+      <c r="BQ19" s="104"/>
+      <c r="BR19" s="104"/>
+      <c r="BS19" s="104"/>
+      <c r="BT19" s="104"/>
+      <c r="BU19" s="104"/>
+      <c r="BV19" s="104"/>
+      <c r="BW19" s="104"/>
+      <c r="BX19" s="104"/>
+      <c r="BY19" s="104"/>
+      <c r="BZ19" s="104"/>
+      <c r="CA19" s="104"/>
+      <c r="CB19" s="104"/>
+      <c r="CC19" s="104"/>
+      <c r="CD19" s="104"/>
+      <c r="CE19" s="104"/>
+      <c r="CF19" s="104"/>
+      <c r="CG19" s="103"/>
     </row>
     <row r="20" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG20" s="112"/>
+      <c r="CG20" s="103"/>
     </row>
     <row r="21" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG21" s="112"/>
+      <c r="CG21" s="103"/>
     </row>
     <row r="22" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG22" s="112"/>
+      <c r="CG22" s="103"/>
     </row>
     <row r="23" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG23" s="112"/>
+      <c r="CG23" s="103"/>
     </row>
     <row r="24" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG24" s="112"/>
+      <c r="CG24" s="103"/>
     </row>
     <row r="25" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG25" s="112"/>
+      <c r="CG25" s="103"/>
     </row>
     <row r="26" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG26" s="112"/>
+      <c r="CG26" s="103"/>
     </row>
     <row r="27" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG27" s="112"/>
+      <c r="CG27" s="103"/>
     </row>
     <row r="28" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG28" s="112"/>
+      <c r="CG28" s="103"/>
     </row>
     <row r="29" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG29" s="112"/>
+      <c r="CG29" s="103"/>
     </row>
     <row r="30" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG30" s="112"/>
+      <c r="CG30" s="103"/>
     </row>
     <row r="31" spans="1:85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="CG31" s="112"/>
+      <c r="CG31" s="103"/>
     </row>
     <row r="32" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="CG32" s="112"/>
+      <c r="CG32" s="103"/>
     </row>
     <row r="33" spans="85:85" x14ac:dyDescent="0.2">
-      <c r="CG33" s="112"/>
+      <c r="CG33" s="103"/>
     </row>
     <row r="34" spans="85:85" x14ac:dyDescent="0.2">
-      <c r="CG34" s="112"/>
+      <c r="CG34" s="103"/>
     </row>
     <row r="35" spans="85:85" x14ac:dyDescent="0.2">
-      <c r="CG35" s="112"/>
+      <c r="CG35" s="103"/>
     </row>
     <row r="36" spans="85:85" x14ac:dyDescent="0.2">
-      <c r="CG36" s="112"/>
+      <c r="CG36" s="103"/>
     </row>
     <row r="37" spans="85:85" x14ac:dyDescent="0.2">
-      <c r="CG37" s="112"/>
+      <c r="CG37" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="Y4:AB4"/>
+    <mergeCell ref="E2:AR3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="AS2:CF3"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AO4:AR4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="AS4:AV4"/>
+    <mergeCell ref="AW4:AZ4"/>
+    <mergeCell ref="BU4:BX4"/>
+    <mergeCell ref="BQ4:BT4"/>
+    <mergeCell ref="BY4:CB4"/>
+    <mergeCell ref="CC4:CF4"/>
     <mergeCell ref="E6:H16"/>
     <mergeCell ref="BA6:BD16"/>
     <mergeCell ref="BQ6:BT16"/>
@@ -3767,26 +3790,6 @@
     <mergeCell ref="U6:AB16"/>
     <mergeCell ref="AK6:AN16"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="AS2:CF3"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AO4:AR4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AG4:AJ4"/>
-    <mergeCell ref="AS4:AV4"/>
-    <mergeCell ref="AW4:AZ4"/>
-    <mergeCell ref="BU4:BX4"/>
-    <mergeCell ref="BQ4:BT4"/>
-    <mergeCell ref="BY4:CB4"/>
-    <mergeCell ref="CC4:CF4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="Y4:AB4"/>
-    <mergeCell ref="E2:AR3"/>
-    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="C6:C18">
@@ -3815,6 +3818,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2041c0d2b30335279095007fcb0a9d7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b9c1bb8339570eda07374d036e5caf" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -4027,17 +4041,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4048,6 +4051,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C334E08-C15B-4283-B082-739F59C9FCA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4066,19 +4082,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
   <ds:schemaRefs>

</xml_diff>